<commit_message>
Lernjournal angepasst und Zeit eingetragen
</commit_message>
<xml_diff>
--- a/aufgabe_1+2+3_team_3_lernjournal.xlsx
+++ b/aufgabe_1+2+3_team_3_lernjournal.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="0" windowWidth="26660" windowHeight="18660" tabRatio="350"/>
+    <workbookView xWindow="1240" yWindow="0" windowWidth="26660" windowHeight="18660" tabRatio="415"/>
   </bookViews>
   <sheets>
-    <sheet name="Lernjournal Aufgabe 2" sheetId="2" r:id="rId1"/>
-    <sheet name="Lernjournal Aufgabe 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Lernjournal Aufgabe 3" sheetId="3" r:id="rId1"/>
+    <sheet name="Lernjournal Aufgabe 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Lernjournal Aufgabe 1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="31">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -137,6 +138,9 @@
   </si>
   <si>
     <t>Finish der gemiensamen Korrekturen und Layout ausputzen/fehler beheben</t>
+  </si>
+  <si>
+    <t>Dokument angepasst. Neue Aufgabenstellunge eingebaut und Lyout angepasst.</t>
   </si>
 </sst>
 </file>
@@ -744,7 +748,7 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -949,16 +953,10 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="21">
-        <v>120</v>
-      </c>
-      <c r="C11" s="22">
-        <v>41385</v>
-      </c>
+    <row r="11" spans="1:16" s="11" customFormat="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -973,16 +971,10 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A12" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="21">
-        <v>90</v>
-      </c>
-      <c r="C12" s="22">
-        <v>41385</v>
-      </c>
+    <row r="12" spans="1:16" s="11" customFormat="1">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -997,16 +989,10 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="36">
-      <c r="A13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="21">
-        <v>105</v>
-      </c>
-      <c r="C13" s="22">
-        <v>41388</v>
-      </c>
+    <row r="13" spans="1:16" s="11" customFormat="1">
+      <c r="A13" s="8"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -1022,15 +1008,9 @@
       <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16" s="11" customFormat="1">
-      <c r="A14" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="8">
-        <v>15</v>
-      </c>
-      <c r="C14" s="9">
-        <v>41389</v>
-      </c>
+      <c r="A14" s="20"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -1046,15 +1026,9 @@
       <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:16" s="11" customFormat="1">
-      <c r="A15" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="8">
-        <v>45</v>
-      </c>
-      <c r="C15" s="9">
-        <v>41390</v>
-      </c>
+      <c r="A15" s="20"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1093,11 +1067,11 @@
       </c>
       <c r="B17" s="18">
         <f>SUM(B11:B16)</f>
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="C17" s="19">
         <f>TIME(0,B17,)</f>
-        <v>0.26041666666666669</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1231,15 +1205,15 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+    <row r="24" spans="1:16" s="11" customFormat="1">
       <c r="A24" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="24">
         <v>25</v>
       </c>
-      <c r="B24" s="24">
-        <v>40</v>
-      </c>
       <c r="C24" s="25">
-        <v>41384</v>
+        <v>41433</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -1256,15 +1230,9 @@
       <c r="P24" s="10"/>
     </row>
     <row r="25" spans="1:16" s="11" customFormat="1">
-      <c r="A25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="21">
-        <v>75</v>
-      </c>
-      <c r="C25" s="22">
-        <v>41385</v>
-      </c>
+      <c r="A25" s="8"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -1279,16 +1247,10 @@
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A26" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="21">
-        <v>120</v>
-      </c>
-      <c r="C26" s="22">
-        <v>41385</v>
-      </c>
+    <row r="26" spans="1:16" s="11" customFormat="1">
+      <c r="A26" s="8"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -1304,15 +1266,9 @@
       <c r="P26" s="10"/>
     </row>
     <row r="27" spans="1:16" s="11" customFormat="1">
-      <c r="A27" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="21">
-        <v>65</v>
-      </c>
-      <c r="C27" s="22">
-        <v>41385</v>
-      </c>
+      <c r="A27" s="8"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -1327,16 +1283,10 @@
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
     </row>
-    <row r="28" spans="1:16" s="11" customFormat="1" ht="36">
-      <c r="A28" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="21">
-        <v>105</v>
-      </c>
-      <c r="C28" s="22">
-        <v>41388</v>
-      </c>
+    <row r="28" spans="1:16" s="11" customFormat="1">
+      <c r="A28" s="8"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -1352,15 +1302,9 @@
       <c r="P28" s="10"/>
     </row>
     <row r="29" spans="1:16" s="11" customFormat="1">
-      <c r="A29" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="24">
-        <v>30</v>
-      </c>
-      <c r="C29" s="25">
-        <v>41389</v>
-      </c>
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -1376,15 +1320,9 @@
       <c r="P29" s="10"/>
     </row>
     <row r="30" spans="1:16" s="11" customFormat="1">
-      <c r="A30" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="24">
-        <v>45</v>
-      </c>
-      <c r="C30" s="25">
-        <v>41390</v>
-      </c>
+      <c r="A30" s="20"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -1400,15 +1338,9 @@
       <c r="P30" s="10"/>
     </row>
     <row r="31" spans="1:16" s="11" customFormat="1">
-      <c r="A31" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="24">
-        <v>25</v>
-      </c>
-      <c r="C31" s="25">
-        <v>41399</v>
-      </c>
+      <c r="A31" s="20"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -1447,11 +1379,11 @@
       </c>
       <c r="B33" s="18">
         <f>SUM(B24:B32)</f>
-        <v>505</v>
+        <v>25</v>
       </c>
       <c r="C33" s="19">
         <f>TIME(0,B33,)</f>
-        <v>0.35069444444444442</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1680,11 +1612,11 @@
       </c>
       <c r="B45" s="16">
         <f>SUM(B33,B17)</f>
-        <v>880</v>
+        <v>25</v>
       </c>
       <c r="C45" s="17">
         <f>TIME(0,B45,)</f>
-        <v>0.61111111111111105</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1723,6 +1655,988 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" s="4" customFormat="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" s="4" customFormat="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" s="4" customFormat="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" s="4" customFormat="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" s="4" customFormat="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" s="4" customFormat="1">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="21">
+        <v>120</v>
+      </c>
+      <c r="C11" s="22">
+        <v>41385</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+    </row>
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A12" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="21">
+        <v>90</v>
+      </c>
+      <c r="C12" s="22">
+        <v>41385</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="21">
+        <v>105</v>
+      </c>
+      <c r="C13" s="22">
+        <v>41388</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="1:16" s="11" customFormat="1">
+      <c r="A14" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="8">
+        <v>15</v>
+      </c>
+      <c r="C14" s="9">
+        <v>41389</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+    </row>
+    <row r="15" spans="1:16" s="11" customFormat="1">
+      <c r="A15" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="8">
+        <v>45</v>
+      </c>
+      <c r="C15" s="9">
+        <v>41390</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="1:16" s="4" customFormat="1">
+      <c r="A17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="18">
+        <f>SUM(B11:B16)</f>
+        <v>375</v>
+      </c>
+      <c r="C17" s="19">
+        <f>TIME(0,B17,)</f>
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" s="4" customFormat="1">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" s="4" customFormat="1">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" s="4" customFormat="1">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" s="4" customFormat="1">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" s="4" customFormat="1">
+      <c r="A23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A24" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="24">
+        <v>40</v>
+      </c>
+      <c r="C24" s="25">
+        <v>41384</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+    </row>
+    <row r="25" spans="1:16" s="11" customFormat="1">
+      <c r="A25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="21">
+        <v>75</v>
+      </c>
+      <c r="C25" s="22">
+        <v>41385</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+    </row>
+    <row r="26" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A26" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="21">
+        <v>120</v>
+      </c>
+      <c r="C26" s="22">
+        <v>41385</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+    </row>
+    <row r="27" spans="1:16" s="11" customFormat="1">
+      <c r="A27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="21">
+        <v>65</v>
+      </c>
+      <c r="C27" s="22">
+        <v>41385</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+    </row>
+    <row r="28" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A28" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="21">
+        <v>105</v>
+      </c>
+      <c r="C28" s="22">
+        <v>41388</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+    </row>
+    <row r="29" spans="1:16" s="11" customFormat="1">
+      <c r="A29" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="24">
+        <v>30</v>
+      </c>
+      <c r="C29" s="25">
+        <v>41389</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+    </row>
+    <row r="30" spans="1:16" s="11" customFormat="1">
+      <c r="A30" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="24">
+        <v>45</v>
+      </c>
+      <c r="C30" s="25">
+        <v>41390</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+    </row>
+    <row r="31" spans="1:16" s="11" customFormat="1">
+      <c r="A31" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="24">
+        <v>25</v>
+      </c>
+      <c r="C31" s="25">
+        <v>41399</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+    </row>
+    <row r="32" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+    </row>
+    <row r="33" spans="1:16" s="4" customFormat="1">
+      <c r="A33" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="18">
+        <f>SUM(B24:B32)</f>
+        <v>505</v>
+      </c>
+      <c r="C33" s="19">
+        <f>TIME(0,B33,)</f>
+        <v>0.35069444444444442</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="1:16" s="4" customFormat="1">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+    </row>
+    <row r="37" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
+      <c r="A37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A39" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+    </row>
+    <row r="40" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A40" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="8">
+        <v>0</v>
+      </c>
+      <c r="C40" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+    </row>
+    <row r="41" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A41" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="8">
+        <v>0</v>
+      </c>
+      <c r="C41" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+    </row>
+    <row r="42" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+    </row>
+    <row r="43" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A43" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="14">
+        <f>SUM(B40:B42)</f>
+        <v>0</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+    </row>
+    <row r="45" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
+      <c r="A45" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="16">
+        <f>SUM(B33,B17)</f>
+        <v>880</v>
+      </c>
+      <c r="C45" s="17">
+        <f>TIME(0,B45,)</f>
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.2" right="0.2" top="0.41000000000000009" bottom="0.41000000000000009" header="0.2" footer="0.2"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial,Bold"&amp;8Technikerschule HF Zürich – Informatik&amp;C&amp;"Arial,Bold"&amp;8Software Engineering&amp;R&amp;"Arial,Bold"&amp;8Semesterprojekt - Lernjournal</oddHeader>
+    <oddFooter>&amp;L&amp;"Arial,Bold"&amp;8&amp;D&amp;C&amp;"Arial,Bold"&amp;8&amp;P/&amp;N&amp;R&amp;"Arial,Bold"&amp;8Arif Chughtai</oddFooter>
+  </headerFooter>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="3" max="1048575" man="1"/>
+  </colBreaks>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Fachklassendiagram zwei Versionen erfasst. Pages Dokument um Fachbegriff-Glossar Tabellen erweitert. Lernjournal ergänzt
</commit_message>
<xml_diff>
--- a/aufgabe_1+2+3_team_3_lernjournal.xlsx
+++ b/aufgabe_1+2+3_team_3_lernjournal.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>Korrekturen erster Teil, soweit möglich, eingearbeit.</t>
+  </si>
+  <si>
+    <t>Fachklassendiagramm erstellt (inkl. Besprechung bei der Arbeit über das Wie?)!</t>
+  </si>
+  <si>
+    <t>Anwendungsfall Diagramm angepasst - neue Version / Ideen</t>
   </si>
 </sst>
 </file>
@@ -751,7 +757,7 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1257,9 +1263,15 @@
       <c r="P25" s="10"/>
     </row>
     <row r="26" spans="1:16" s="11" customFormat="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
+      <c r="A26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="21">
+        <v>50</v>
+      </c>
+      <c r="C26" s="22">
+        <v>41440</v>
+      </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -1275,9 +1287,15 @@
       <c r="P26" s="10"/>
     </row>
     <row r="27" spans="1:16" s="11" customFormat="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
+      <c r="A27" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="21">
+        <v>15</v>
+      </c>
+      <c r="C27" s="22">
+        <v>41439</v>
+      </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -1388,11 +1406,11 @@
       </c>
       <c r="B33" s="18">
         <f>SUM(B24:B32)</f>
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="C33" s="19">
         <f>TIME(0,B33,)</f>
-        <v>3.125E-2</v>
+        <v>7.6388888888888881E-2</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1621,11 +1639,11 @@
       </c>
       <c r="B45" s="16">
         <f>SUM(B33,B17)</f>
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="C45" s="17">
         <f>TIME(0,B45,)</f>
-        <v>3.125E-2</v>
+        <v>7.6388888888888881E-2</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>

</xml_diff>

<commit_message>
Fachklassendiagramm zusammgeführt,Glosser erstellt (so gut möglich) und Lernjournal angepasst. Ein bitzeli aufgeräumt
</commit_message>
<xml_diff>
--- a/aufgabe_1+2+3_team_3_lernjournal.xlsx
+++ b/aufgabe_1+2+3_team_3_lernjournal.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="415"/>
+    <workbookView xWindow="940" yWindow="620" windowWidth="29720" windowHeight="18940" tabRatio="415"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal Aufgabe 3" sheetId="3" r:id="rId1"/>
     <sheet name="Lernjournal Aufgabe 2" sheetId="2" r:id="rId2"/>
     <sheet name="Lernjournal Aufgabe 1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -158,16 +163,19 @@
   <si>
     <t>Fachklassendiagramm ( Aufgabe 1 ) erstellt - 2 und 3 Version - Vorschlag</t>
   </si>
+  <si>
+    <t>Fachklassendiagramm zusammengeführt - Vereinheitlicht, Versucht richtige Lösung für das Glosser zu finden. Begriffe nach unserem Verständniss der Aufgabenstellung definiert und beschreiben.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="???\ &quot;Minuten&quot;"/>
     <numFmt numFmtId="165" formatCode="[hh]:mm\ &quot;Std:Min&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -279,8 +287,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -427,9 +439,6 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -445,76 +454,83 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="69">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+  <cellStyles count="73">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -843,20 +859,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -877,11 +893,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -932,7 +948,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -988,7 +1004,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1028,7 +1044,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="10" spans="1:16" s="4" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1053,13 +1069,13 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" s="11" customFormat="1">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="29">
         <v>45</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="30">
         <v>41434</v>
       </c>
       <c r="D11" s="10"/>
@@ -1077,13 +1093,13 @@
       <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:16" s="11" customFormat="1">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="29">
         <v>5</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="30">
         <v>41434</v>
       </c>
       <c r="D12" s="10"/>
@@ -1101,13 +1117,13 @@
       <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:16" s="11" customFormat="1">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="29">
         <v>45</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="30">
         <v>41434</v>
       </c>
       <c r="D13" s="10"/>
@@ -1125,13 +1141,13 @@
       <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16" s="11" customFormat="1">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="26">
         <v>30</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="27">
         <v>41436</v>
       </c>
       <c r="D14" s="10"/>
@@ -1148,10 +1164,1016 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A15" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="26">
+        <v>105</v>
+      </c>
+      <c r="C15" s="27">
+        <v>41441</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="1:16" s="11" customFormat="1">
+      <c r="A16" s="28"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="1:16" s="11" customFormat="1">
+      <c r="A17" s="20"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="1:16" s="4" customFormat="1">
+      <c r="A19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="18">
+        <f>SUM(B11:B18)</f>
+        <v>230</v>
+      </c>
+      <c r="C19" s="19">
+        <f>TIME(0,B19,)</f>
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" s="4" customFormat="1">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" s="4" customFormat="1">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" s="4" customFormat="1">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" s="4" customFormat="1">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" s="4" customFormat="1">
+      <c r="A25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" s="11" customFormat="1">
+      <c r="A26" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="24">
+        <v>20</v>
+      </c>
+      <c r="C26" s="25">
+        <v>41433</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+    </row>
+    <row r="27" spans="1:16" s="11" customFormat="1">
+      <c r="A27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="21">
+        <v>25</v>
+      </c>
+      <c r="C27" s="22">
+        <v>41434</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+    </row>
+    <row r="28" spans="1:16" s="11" customFormat="1">
+      <c r="A28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="21">
+        <v>50</v>
+      </c>
+      <c r="C28" s="22">
+        <v>41440</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+    </row>
+    <row r="29" spans="1:16" s="11" customFormat="1">
+      <c r="A29" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="21">
+        <v>15</v>
+      </c>
+      <c r="C29" s="22">
+        <v>41439</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+    </row>
+    <row r="30" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A30" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="26">
+        <v>105</v>
+      </c>
+      <c r="C30" s="27">
+        <v>41441</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+    </row>
+    <row r="31" spans="1:16" s="11" customFormat="1">
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+    </row>
+    <row r="32" spans="1:16" s="11" customFormat="1">
+      <c r="A32" s="20"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+    </row>
+    <row r="33" spans="1:16" s="11" customFormat="1">
+      <c r="A33" s="20"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+    </row>
+    <row r="34" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+    </row>
+    <row r="35" spans="1:16" s="4" customFormat="1">
+      <c r="A35" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="18">
+        <f>SUM(B26:B34)</f>
+        <v>215</v>
+      </c>
+      <c r="C35" s="19">
+        <f>TIME(0,B35,)</f>
+        <v>0.14930555555555555</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" s="4" customFormat="1">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+    </row>
+    <row r="37" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
+      <c r="A39" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+    </row>
+    <row r="40" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+    </row>
+    <row r="41" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A41" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+    </row>
+    <row r="42" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A42" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="8">
+        <v>0</v>
+      </c>
+      <c r="C42" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+    </row>
+    <row r="43" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A43" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="8">
+        <v>0</v>
+      </c>
+      <c r="C43" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+    </row>
+    <row r="44" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+    </row>
+    <row r="45" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A45" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="14">
+        <f>SUM(B42:B44)</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+    </row>
+    <row r="47" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
+      <c r="A47" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="16">
+        <f>SUM(B35,B19)</f>
+        <v>445</v>
+      </c>
+      <c r="C47" s="17">
+        <f>TIME(0,B47,)</f>
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.2" right="0.2" top="0.41000000000000009" bottom="0.41000000000000009" header="0.2" footer="0.2"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial,Bold"&amp;8Technikerschule HF Zürich – Informatik&amp;C&amp;"Arial,Bold"&amp;8Software Engineering&amp;R&amp;"Arial,Bold"&amp;8Semesterprojekt - Lernjournal</oddHeader>
+    <oddFooter>&amp;L&amp;"Arial,Bold"&amp;8&amp;D&amp;C&amp;"Arial,Bold"&amp;8&amp;P/&amp;N&amp;R&amp;"Arial,Bold"&amp;8Arif Chughtai</oddFooter>
+  </headerFooter>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="3" max="1048575" man="1"/>
+  </colBreaks>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" s="4" customFormat="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" s="4" customFormat="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" s="4" customFormat="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" s="4" customFormat="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" s="4" customFormat="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" s="4" customFormat="1">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="21">
+        <v>120</v>
+      </c>
+      <c r="C11" s="22">
+        <v>41385</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+    </row>
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A12" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="21">
+        <v>90</v>
+      </c>
+      <c r="C12" s="22">
+        <v>41385</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="21">
+        <v>105</v>
+      </c>
+      <c r="C13" s="22">
+        <v>41388</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="1:16" s="11" customFormat="1">
+      <c r="A14" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="8">
+        <v>15</v>
+      </c>
+      <c r="C14" s="9">
+        <v>41389</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+    </row>
     <row r="15" spans="1:16" s="11" customFormat="1">
-      <c r="A15" s="20"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
+      <c r="A15" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="8">
+        <v>45</v>
+      </c>
+      <c r="C15" s="9">
+        <v>41390</v>
+      </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1190,11 +2212,11 @@
       </c>
       <c r="B17" s="18">
         <f>SUM(B11:B16)</f>
-        <v>125</v>
+        <v>375</v>
       </c>
       <c r="C17" s="19">
         <f>TIME(0,B17,)</f>
-        <v>8.6805555555555566E-2</v>
+        <v>0.26041666666666669</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1264,7 +2286,7 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="21" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
@@ -1304,7 +2326,7 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="23" spans="1:16" s="4" customFormat="1">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -1328,15 +2350,15 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="1:16" s="11" customFormat="1" ht="25.5">
+    <row r="24" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
       <c r="A24" s="23" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B24" s="24">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C24" s="25">
-        <v>41433</v>
+        <v>41384</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -1354,13 +2376,13 @@
     </row>
     <row r="25" spans="1:16" s="11" customFormat="1">
       <c r="A25" s="8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B25" s="21">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="C25" s="22">
-        <v>41434</v>
+        <v>41385</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -1376,15 +2398,15 @@
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="1:16" s="11" customFormat="1" ht="25.5">
+    <row r="26" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B26" s="21">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C26" s="22">
-        <v>41440</v>
+        <v>41385</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -1402,13 +2424,13 @@
     </row>
     <row r="27" spans="1:16" s="11" customFormat="1">
       <c r="A27" s="8" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B27" s="21">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="C27" s="22">
-        <v>41439</v>
+        <v>41385</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -1424,10 +2446,16 @@
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
     </row>
-    <row r="28" spans="1:16" s="11" customFormat="1">
-      <c r="A28" s="8"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
+    <row r="28" spans="1:16" s="11" customFormat="1" ht="36">
+      <c r="A28" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="21">
+        <v>105</v>
+      </c>
+      <c r="C28" s="22">
+        <v>41388</v>
+      </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -1443,9 +2471,15 @@
       <c r="P28" s="10"/>
     </row>
     <row r="29" spans="1:16" s="11" customFormat="1">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
+      <c r="A29" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="24">
+        <v>30</v>
+      </c>
+      <c r="C29" s="25">
+        <v>41389</v>
+      </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -1461,9 +2495,15 @@
       <c r="P29" s="10"/>
     </row>
     <row r="30" spans="1:16" s="11" customFormat="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
+      <c r="A30" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="24">
+        <v>45</v>
+      </c>
+      <c r="C30" s="25">
+        <v>41390</v>
+      </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -1479,9 +2519,15 @@
       <c r="P30" s="10"/>
     </row>
     <row r="31" spans="1:16" s="11" customFormat="1">
-      <c r="A31" s="20"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="24">
+        <v>25</v>
+      </c>
+      <c r="C31" s="25">
+        <v>41399</v>
+      </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -1520,11 +2566,11 @@
       </c>
       <c r="B33" s="18">
         <f>SUM(B24:B32)</f>
-        <v>110</v>
+        <v>505</v>
       </c>
       <c r="C33" s="19">
         <f>TIME(0,B33,)</f>
-        <v>7.6388888888888881E-2</v>
+        <v>0.35069444444444442</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1594,7 +2640,7 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
     </row>
-    <row r="37" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
+    <row r="37" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -1634,7 +2680,7 @@
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
     </row>
-    <row r="39" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
+    <row r="39" spans="1:16" s="4" customFormat="1" hidden="1">
       <c r="A39" s="6" t="s">
         <v>4</v>
       </c>
@@ -1747,984 +2793,7 @@
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
     </row>
-    <row r="45" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A45" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" s="16">
-        <f>SUM(B33,B17)</f>
-        <v>235</v>
-      </c>
-      <c r="C45" s="17">
-        <f>TIME(0,B45,)</f>
-        <v>0.16319444444444445</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:C2"/>
-  </mergeCells>
-  <pageMargins left="0.2" right="0.2" top="0.41000000000000009" bottom="0.41000000000000009" header="0.2" footer="0.2"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"Arial,Bold"&amp;8Technikerschule HF Zürich – Informatik&amp;C&amp;"Arial,Bold"&amp;8Software Engineering&amp;R&amp;"Arial,Bold"&amp;8Semesterprojekt - Lernjournal</oddHeader>
-    <oddFooter>&amp;L&amp;"Arial,Bold"&amp;8&amp;D&amp;C&amp;"Arial,Bold"&amp;8&amp;P/&amp;N&amp;R&amp;"Arial,Bold"&amp;8Arif Chughtai</oddFooter>
-  </headerFooter>
-  <colBreaks count="1" manualBreakCount="1">
-    <brk id="3" max="1048575" man="1"/>
-  </colBreaks>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P45"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" s="4" customFormat="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" s="4" customFormat="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
-      <c r="A5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" s="4" customFormat="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" s="4" customFormat="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
-      <c r="A8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" s="4" customFormat="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
-      <c r="A10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="21">
-        <v>120</v>
-      </c>
-      <c r="C11" s="22">
-        <v>41385</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-    </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A12" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="21">
-        <v>90</v>
-      </c>
-      <c r="C12" s="22">
-        <v>41385</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-    </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="38.25">
-      <c r="A13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="21">
-        <v>105</v>
-      </c>
-      <c r="C13" s="22">
-        <v>41388</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-    </row>
-    <row r="14" spans="1:16" s="11" customFormat="1">
-      <c r="A14" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="8">
-        <v>15</v>
-      </c>
-      <c r="C14" s="9">
-        <v>41389</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-    </row>
-    <row r="15" spans="1:16" s="11" customFormat="1">
-      <c r="A15" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="8">
-        <v>45</v>
-      </c>
-      <c r="C15" s="9">
-        <v>41390</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-    </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-    </row>
-    <row r="17" spans="1:16" s="4" customFormat="1">
-      <c r="A17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="18">
-        <f>SUM(B11:B16)</f>
-        <v>375</v>
-      </c>
-      <c r="C17" s="19">
-        <f>TIME(0,B17,)</f>
-        <v>0.26041666666666669</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="1:16" s="4" customFormat="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="1:16" s="4" customFormat="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="1:16" s="4" customFormat="1">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="1:16" s="4" customFormat="1" ht="15.75">
-      <c r="A21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-    </row>
-    <row r="22" spans="1:16" s="4" customFormat="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-    </row>
-    <row r="23" spans="1:16" s="4" customFormat="1" ht="25.5">
-      <c r="A23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-    </row>
-    <row r="24" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A24" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="24">
-        <v>40</v>
-      </c>
-      <c r="C24" s="25">
-        <v>41384</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-    </row>
-    <row r="25" spans="1:16" s="11" customFormat="1">
-      <c r="A25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="21">
-        <v>75</v>
-      </c>
-      <c r="C25" s="22">
-        <v>41385</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-    </row>
-    <row r="26" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A26" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="21">
-        <v>120</v>
-      </c>
-      <c r="C26" s="22">
-        <v>41385</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-    </row>
-    <row r="27" spans="1:16" s="11" customFormat="1" ht="25.5">
-      <c r="A27" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="21">
-        <v>65</v>
-      </c>
-      <c r="C27" s="22">
-        <v>41385</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-    </row>
-    <row r="28" spans="1:16" s="11" customFormat="1" ht="38.25">
-      <c r="A28" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="21">
-        <v>105</v>
-      </c>
-      <c r="C28" s="22">
-        <v>41388</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-    </row>
-    <row r="29" spans="1:16" s="11" customFormat="1">
-      <c r="A29" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="24">
-        <v>30</v>
-      </c>
-      <c r="C29" s="25">
-        <v>41389</v>
-      </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-    </row>
-    <row r="30" spans="1:16" s="11" customFormat="1">
-      <c r="A30" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="24">
-        <v>45</v>
-      </c>
-      <c r="C30" s="25">
-        <v>41390</v>
-      </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-    </row>
-    <row r="31" spans="1:16" s="11" customFormat="1">
-      <c r="A31" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="24">
-        <v>25</v>
-      </c>
-      <c r="C31" s="25">
-        <v>41399</v>
-      </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-    </row>
-    <row r="32" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-    </row>
-    <row r="33" spans="1:16" s="4" customFormat="1">
-      <c r="A33" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="18">
-        <f>SUM(B24:B32)</f>
-        <v>505</v>
-      </c>
-      <c r="C33" s="19">
-        <f>TIME(0,B33,)</f>
-        <v>0.35069444444444442</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-    </row>
-    <row r="34" spans="1:16" s="4" customFormat="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-    </row>
-    <row r="35" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-    </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-    </row>
-    <row r="37" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
-      <c r="A37" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-    </row>
-    <row r="38" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-    </row>
-    <row r="39" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
-      <c r="A39" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-    </row>
-    <row r="40" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A40" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="8">
-        <v>0</v>
-      </c>
-      <c r="C40" s="9">
-        <v>41275</v>
-      </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-    </row>
-    <row r="41" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A41" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="8">
-        <v>0</v>
-      </c>
-      <c r="C41" s="9">
-        <v>41275</v>
-      </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-    </row>
-    <row r="42" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-    </row>
-    <row r="43" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A43" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43" s="14">
-        <f>SUM(B40:B42)</f>
-        <v>0</v>
-      </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-    </row>
-    <row r="45" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="45" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
       <c r="A45" s="15" t="s">
         <v>15</v>
       </c>
@@ -2772,20 +2841,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2806,11 +2875,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2861,7 +2930,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -2917,7 +2986,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2957,7 +3026,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="10" spans="1:16" s="4" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -3172,7 +3241,7 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" s="4" customFormat="1" ht="15.75">
+    <row r="20" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
@@ -3212,7 +3281,7 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1" ht="25.5">
+    <row r="22" spans="1:16" s="4" customFormat="1">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
@@ -3475,7 +3544,7 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" s="4" customFormat="1" ht="15.75" hidden="1">
+    <row r="34" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
       <c r="A34" s="5" t="s">
         <v>2</v>
       </c>
@@ -3515,7 +3584,7 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" ht="25.5" hidden="1">
+    <row r="36" spans="1:16" s="4" customFormat="1" hidden="1">
       <c r="A36" s="6" t="s">
         <v>4</v>
       </c>
@@ -3628,7 +3697,7 @@
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
     </row>
-    <row r="42" spans="1:16" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
       <c r="A42" s="15" t="s">
         <v>15</v>
       </c>

</xml_diff>